<commit_message>
changed the data viz picture to a higher res
</commit_message>
<xml_diff>
--- a/Analysis_Worksheets/cryptopunks.xlsx
+++ b/Analysis_Worksheets/cryptopunks.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cryptopunks\AnalysisWorksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Analysis_of_Cryptopunks_Top_60\Analysis_Worksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A01751E-3140-4422-94FA-AE0CCC2005A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F35B62-2772-4E88-9E71-26A56EA8ACE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_xltb_storage_" sheetId="5" state="veryHidden" r:id="rId1"/>
     <sheet name="Data viz" sheetId="4" r:id="rId2"/>
-    <sheet name="cryptopunks" sheetId="1" r:id="rId3"/>
-    <sheet name="attributes" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="cryptopunks" sheetId="1" r:id="rId4"/>
+    <sheet name="attributes" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">attributes!$B$1:$B$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">attributes!$B$1:$B$101</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1094,6 +1095,12 @@
     <t>XLToolbox.Export.Models.BatchExportSettings</t>
   </si>
   <si>
+    <t>export_path</t>
+  </si>
+  <si>
+    <t>cheapest (Ξ)</t>
+  </si>
+  <si>
     <t>&lt;?xml version="1.0" encoding="utf-16"?&gt;_x000D_
 &lt;BatchExportSettings xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance"&gt;_x000D_
   &lt;Preset&gt;_x000D_
@@ -1109,18 +1116,12 @@
   &lt;Scope&gt;ActiveSheet&lt;/Scope&gt;_x000D_
   &lt;Objects&gt;ChartsAndShapes&lt;/Objects&gt;_x000D_
   &lt;Layout&gt;SheetLayout&lt;/Layout&gt;_x000D_
-  &lt;Path&gt;C:\cryptopunks&lt;/Path&gt;_x000D_
-  &lt;Screenshot&gt;false&lt;/Screenshot&gt;_x000D_
+  &lt;Path&gt;C:\Users\DELL\OneDrive\Documents&lt;/Path&gt;_x000D_
+  &lt;Screenshot&gt;true&lt;/Screenshot&gt;_x000D_
 &lt;/BatchExportSettings&gt;</t>
   </si>
   <si>
-    <t>export_path</t>
-  </si>
-  <si>
-    <t>C:\cryptopunks\data-viz.png</t>
-  </si>
-  <si>
-    <t>cheapest (Ξ)</t>
+    <t>C:\Analysis_of_Cryptopunks_Top_60\data-viz.png</t>
   </si>
 </sst>
 </file>
@@ -2480,7 +2481,7 @@
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1332142416"/>
@@ -5750,13 +5751,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>4581071</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>2548</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>8373421</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>178377</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5788,13 +5789,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>4577195</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>11546</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>8367995</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>2964</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5826,13 +5827,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>219364</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>14942</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1824182</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>14942</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -5848,7 +5849,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="219364" y="2523192"/>
+          <a:off x="219364" y="2300942"/>
           <a:ext cx="1604818" cy="1143000"/>
           <a:chOff x="6021294" y="11586883"/>
           <a:chExt cx="1837850" cy="1234004"/>
@@ -5982,193 +5983,17 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>3175</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2035176</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>96</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89174C6C-B9BA-F7B9-5118-4106BB2585C4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="5271" r="6626"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="177800" y="719585"/>
-          <a:ext cx="1857376" cy="1413460"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2216150</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2216150</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1339850</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="Straight Connector 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22D69CBB-9ECA-ECF0-4FAE-CC3CD125FF57}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2216150" y="425450"/>
-          <a:ext cx="0" cy="1276350"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2273300</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>8534400</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1308100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="TextBox 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E14DF7F-41AB-B6C1-E14B-722E2F3C94D3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2273300" y="460188"/>
-          <a:ext cx="6261100" cy="1206500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="just"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200"/>
-            <a:t>An NFT Collection launched in 2017, Cryptopunks are credited with starting</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0"/>
-            <a:t> the NFT Craze of 2021. There are 10,000 CryptoPunks in general and are classified based on punk types: Ape, Alien, Female, Male and Zombie; Attributes they possess and Attribute Counts . This project was carried out to analyse if the price a punk is sold at depends on rarity of a punk type or attribute count.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2401511</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>7816</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>4007111</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>8252</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -6184,7 +6009,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2401511" y="2516066"/>
+          <a:off x="2401511" y="2293816"/>
           <a:ext cx="1605600" cy="1143436"/>
           <a:chOff x="6021297" y="11586883"/>
           <a:chExt cx="1763059" cy="1135530"/>
@@ -6318,13 +6143,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>219728</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>10525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>4020657</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>5763</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6333,6 +6158,44 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F0AE41E-78E7-4D79-B183-EB59B70DD0B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219392</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>10153</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4020992</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>7485</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="42" name="Chart 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6436C39-2B41-4F2E-8069-E1B52894503B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6355,52 +6218,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>219392</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>10153</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4020992</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>7485</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="42" name="Chart 41">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6436C39-2B41-4F2E-8069-E1B52894503B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>242454</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>10539</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1764467</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>183986</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6416,7 +6241,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="242454" y="3058539"/>
+          <a:off x="242454" y="2868039"/>
           <a:ext cx="1522013" cy="173447"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6465,13 +6290,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2441370</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>176957</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3904095</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>180687</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6487,8 +6312,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2441370" y="2685207"/>
-          <a:ext cx="1462725" cy="187880"/>
+          <a:off x="2441370" y="2843957"/>
+          <a:ext cx="1462725" cy="194230"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6535,1245 +6360,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>335177</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>149001</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>782226</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>33093</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="60" name="Group 59">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A83BDF5-2030-4BA6-A99C-AA29ED28D1F8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="335177" y="4371751"/>
-          <a:ext cx="447049" cy="1789092"/>
-          <a:chOff x="359403" y="3916320"/>
-          <a:chExt cx="447049" cy="1721477"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="61" name="Group 60">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D9D2334-F845-D9AC-B942-6159DB805F54}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="361156" y="3916320"/>
-            <a:ext cx="444500" cy="339851"/>
-            <a:chOff x="361156" y="3924372"/>
-            <a:chExt cx="444500" cy="341673"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="74" name="Picture 73">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9ABC5715-CFF4-EAAE-8394-654979A35186}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="497052" y="3982672"/>
-              <a:ext cx="179519" cy="256329"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="75" name="Rectangle 74">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B9B9AEB-2F64-6AE1-007E-388D8D283905}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="361156" y="3924372"/>
-              <a:ext cx="444500" cy="341673"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="62" name="Group 61">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EECC4AB2-E441-7134-F714-5F21897DFEBF}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="359403" y="4256171"/>
-            <a:ext cx="444500" cy="345408"/>
-            <a:chOff x="362745" y="4256768"/>
-            <a:chExt cx="444500" cy="345169"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="72" name="Picture 71">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{658110B3-D934-DD66-3C62-7CE033927BF2}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="508000" y="4288518"/>
-              <a:ext cx="162903" cy="254268"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="73" name="Rectangle 72">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89A6A910-D7C9-564A-F257-17BFF99E8F70}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="362745" y="4256768"/>
-              <a:ext cx="444500" cy="345169"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="63" name="Group 62">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1593F1C-49B6-31BA-D473-CB22939A99D1}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="360364" y="4602204"/>
-            <a:ext cx="444500" cy="345407"/>
-            <a:chOff x="360364" y="4605904"/>
-            <a:chExt cx="444500" cy="345169"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="70" name="Picture 69">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EE50B4D-E1FB-126F-78D7-9E48B5AB5CE8}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
-              <a:duotone>
-                <a:prstClr val="black"/>
-                <a:srgbClr val="7DA269">
-                  <a:tint val="45000"/>
-                  <a:satMod val="400000"/>
-                </a:srgbClr>
-              </a:duotone>
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="465932" y="4636862"/>
-              <a:ext cx="252000" cy="251546"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="71" name="Rectangle 70">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB064605-AF85-F05E-4BF1-231BB3FCC5F7}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="360364" y="4605904"/>
-              <a:ext cx="444500" cy="345169"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="64" name="Group 63">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93810894-7B93-8CB5-73AE-3C9F97FDD384}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="361952" y="4944895"/>
-            <a:ext cx="444500" cy="345408"/>
-            <a:chOff x="361952" y="4955041"/>
-            <a:chExt cx="444500" cy="345168"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="68" name="Picture 67">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{753C836E-EF25-BC72-3732-D5A06C4D8AE7}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
-              <a:duotone>
-                <a:prstClr val="black"/>
-                <a:srgbClr val="E8D8CA">
-                  <a:tint val="45000"/>
-                  <a:satMod val="400000"/>
-                </a:srgbClr>
-              </a:duotone>
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="487362" y="5007428"/>
-              <a:ext cx="216314" cy="253133"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="69" name="Rectangle 68">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E681DB28-900B-8BB5-C0C0-6164B255F5FF}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="361952" y="4955041"/>
-              <a:ext cx="444500" cy="345168"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="65" name="Group 64">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A64213C2-4EBA-8C30-D382-2DFADCFEBD1F}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="359571" y="5292390"/>
-            <a:ext cx="444500" cy="345407"/>
-            <a:chOff x="359571" y="5292270"/>
-            <a:chExt cx="444500" cy="345169"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="66" name="Picture 65">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84FC4A77-2151-4006-6DC9-8A6E35920B29}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
-              <a:duotone>
-                <a:prstClr val="black"/>
-                <a:srgbClr val="C8FBFB">
-                  <a:tint val="45000"/>
-                  <a:satMod val="400000"/>
-                </a:srgbClr>
-              </a:duotone>
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="488950" y="5332753"/>
-              <a:ext cx="234354" cy="253134"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="67" name="Rectangle 66">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1BE677F-7587-624C-C780-B802948DB094}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="359571" y="5292270"/>
-              <a:ext cx="444500" cy="345169"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4946221</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>20343</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>8005411</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>30228</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="77" name="Group 76">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FD7AD55-3018-A18B-73A7-069575407410}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="4946221" y="5957593"/>
-          <a:ext cx="3059190" cy="390885"/>
-          <a:chOff x="9163969" y="4272977"/>
-          <a:chExt cx="3057219" cy="374320"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="35" name="Group 34">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{647D2041-0D06-8036-DAAA-8C4CC3BCA17C}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="11772790" y="4274122"/>
-            <a:ext cx="448398" cy="336133"/>
-            <a:chOff x="361156" y="3924372"/>
-            <a:chExt cx="444500" cy="341673"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="23" name="Picture 22">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4099F02-F925-50AC-BC5D-C32F099C3B76}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="497052" y="3982672"/>
-              <a:ext cx="179519" cy="256329"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="30" name="Rectangle 29">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F53AD360-D2C3-2068-BFEE-B3D7449B92B7}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="361156" y="3924372"/>
-              <a:ext cx="444500" cy="341673"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="36" name="Group 35">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20028502-B767-F73E-EF26-FD9A7F9C9DAB}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="11136036" y="4305586"/>
-            <a:ext cx="444500" cy="341711"/>
-            <a:chOff x="362745" y="4256768"/>
-            <a:chExt cx="444500" cy="345169"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="29" name="Picture 28">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A3F4A10-6AC7-E89F-C298-A5CDC2BF5ED4}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="508000" y="4288518"/>
-              <a:ext cx="162903" cy="254268"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="31" name="Rectangle 30">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{362ABB6C-2E52-4554-A325-56B8629D6FAD}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="362745" y="4256768"/>
-              <a:ext cx="444500" cy="345169"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="37" name="Group 36">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DF8B5D8-A28C-0D89-107B-BC2BA2950DF4}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="10479586" y="4290958"/>
-            <a:ext cx="444500" cy="341710"/>
-            <a:chOff x="360364" y="4605904"/>
-            <a:chExt cx="444500" cy="345169"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="11" name="Picture 10">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B55B3221-42CC-C1D5-439D-96A9EF4ACE39}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
-              <a:duotone>
-                <a:prstClr val="black"/>
-                <a:srgbClr val="7DA269">
-                  <a:tint val="45000"/>
-                  <a:satMod val="400000"/>
-                </a:srgbClr>
-              </a:duotone>
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="465932" y="4636862"/>
-              <a:ext cx="252000" cy="251546"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="32" name="Rectangle 31">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FC6C50A-0BDD-45FB-B3A7-B0B7873489AC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="360364" y="4605904"/>
-              <a:ext cx="444500" cy="345169"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="38" name="Group 37">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A86E4159-F552-569C-B2C0-15A12A43F80C}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="9808820" y="4272977"/>
-            <a:ext cx="444500" cy="341711"/>
-            <a:chOff x="361952" y="4955041"/>
-            <a:chExt cx="444500" cy="345168"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="13" name="Picture 12">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7FDD080-38CF-626B-0EB7-D503F5B099C4}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
-              <a:duotone>
-                <a:prstClr val="black"/>
-                <a:srgbClr val="E8D8CA">
-                  <a:tint val="45000"/>
-                  <a:satMod val="400000"/>
-                </a:srgbClr>
-              </a:duotone>
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="487362" y="5007428"/>
-              <a:ext cx="216314" cy="253133"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="33" name="Rectangle 32">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EAC67AD-7CA9-41A3-B3A1-330355D347E3}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="361952" y="4955041"/>
-              <a:ext cx="444500" cy="345168"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="39" name="Group 38">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{638BC97F-7984-BEE5-FCF5-DF908284F210}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="9163969" y="4297170"/>
-            <a:ext cx="444500" cy="339672"/>
-            <a:chOff x="359571" y="5292270"/>
-            <a:chExt cx="444500" cy="345169"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="9" name="Picture 8">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{121D4025-79C1-BCF6-0CCB-2FCA9D8A2C87}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
-              <a:duotone>
-                <a:prstClr val="black"/>
-                <a:srgbClr val="C8FBFB">
-                  <a:tint val="45000"/>
-                  <a:satMod val="400000"/>
-                </a:srgbClr>
-              </a:duotone>
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="488950" y="5332753"/>
-              <a:ext cx="234354" cy="253134"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="34" name="Rectangle 33">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A725F3E-56B5-4425-987A-38AAC35FE5AF}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="359571" y="5292270"/>
-              <a:ext cx="444500" cy="345169"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="76" name="Rectangle 75">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3453DB5-F660-1E8C-8196-B292A9548594}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9237870" y="4313662"/>
-            <a:ext cx="2915478" cy="273721"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>4584440</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>19015</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>6189259</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>19451</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -7789,7 +6383,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4584440" y="2527265"/>
+          <a:off x="4584440" y="2305015"/>
           <a:ext cx="1604819" cy="1143436"/>
           <a:chOff x="3635460" y="2163074"/>
           <a:chExt cx="1604819" cy="1121024"/>
@@ -7965,84 +6559,235 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>23091</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>346364</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>29883</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>1397000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="80" name="Rectangle 79">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="41" name="Group 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A80554-514D-BDD6-093A-91A25BE484ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9E6EDC9-C2FE-5B4E-050B-39082B5F5392}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="23091" y="346364"/>
-          <a:ext cx="8573832" cy="1767046"/>
+          <a:off x="23091" y="682625"/>
+          <a:ext cx="8595167" cy="1397000"/>
+          <a:chOff x="23091" y="679824"/>
+          <a:chExt cx="8597968" cy="1397000"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="14" name="Picture 13">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89174C6C-B9BA-F7B9-5118-4106BB2585C4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect l="5271" r="6626"/>
+          <a:stretch/>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="177800" y="682999"/>
+            <a:ext cx="1806575" cy="1371237"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="16" name="Straight Connector 15">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22D69CBB-9ECA-ECF0-4FAE-CC3CD125FF57}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2128837" y="730442"/>
+            <a:ext cx="0" cy="1276350"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="17" name="TextBox 16">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E14DF7F-41AB-B6C1-E14B-722E2F3C94D3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2196353" y="922249"/>
+            <a:ext cx="6338047" cy="885633"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="just"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>An NFT Collection launched in 2017, Cryptopunks are credited with starting</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t> the NFT Craze of 2021. There are 10,000 CryptoPunks in general and are classified based on punk types: Ape, Alien, Female, Male and Zombie; Attributes they possess and Attribute Counts . This project was carried out to analyse if the price a punk is sold at depends on rarity of a punk type or attribute count.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="80" name="Rectangle 79">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A80554-514D-BDD6-093A-91A25BE484ED}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="23091" y="679824"/>
+            <a:ext cx="8597968" cy="1397000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
           <a:noFill/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="50800" dir="2700000" algn="ctr" rotWithShape="0">
-            <a:srgbClr val="638596">
-              <a:alpha val="90000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="50800" dir="2700000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="638596">
+                <a:alpha val="90000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>6766588</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>9778</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>8371407</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>11543</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -8058,7 +6803,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6766588" y="2518028"/>
+          <a:off x="6766588" y="2295778"/>
           <a:ext cx="1604819" cy="1144765"/>
           <a:chOff x="3635460" y="2163074"/>
           <a:chExt cx="1604819" cy="1122368"/>
@@ -8338,13 +7083,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>275937</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>9992</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1080177</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>127880</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -8360,8 +7105,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="275937" y="7306719"/>
-          <a:ext cx="804240" cy="1780434"/>
+          <a:off x="275937" y="7248992"/>
+          <a:ext cx="804240" cy="1832388"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8566,13 +7311,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>4660900</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>8324850</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -8588,8 +7333,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4660900" y="8820150"/>
-          <a:ext cx="3663950" cy="222250"/>
+          <a:off x="4660900" y="8832850"/>
+          <a:ext cx="3663950" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8691,7 +7436,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -8743,6 +7488,1259 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4956969</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>169755</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>8032752</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>179640</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="28" name="Group 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01C95BEB-78D5-4BB7-1D3A-7BEDD9520C5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4956969" y="5694255"/>
+          <a:ext cx="3075783" cy="390885"/>
+          <a:chOff x="9241810" y="4375696"/>
+          <a:chExt cx="3175710" cy="383415"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="77" name="Group 76">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FD7AD55-3018-A18B-73A7-069575407410}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="9241810" y="4375696"/>
+            <a:ext cx="3059190" cy="383415"/>
+            <a:chOff x="9163969" y="4272977"/>
+            <a:chExt cx="3057219" cy="374320"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="30" name="Rectangle 29">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F53AD360-D2C3-2068-BFEE-B3D7449B92B7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11772790" y="4274122"/>
+              <a:ext cx="448398" cy="336133"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="31" name="Rectangle 30">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{362ABB6C-2E52-4554-A325-56B8629D6FAD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11136036" y="4305586"/>
+              <a:ext cx="444500" cy="341711"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="32" name="Rectangle 31">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FC6C50A-0BDD-45FB-B3A7-B0B7873489AC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10479586" y="4290958"/>
+              <a:ext cx="444500" cy="341710"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="33" name="Rectangle 32">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EAC67AD-7CA9-41A3-B3A1-330355D347E3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9808820" y="4272977"/>
+              <a:ext cx="444500" cy="341711"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="34" name="Rectangle 33">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A725F3E-56B5-4425-987A-38AAC35FE5AF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9163969" y="4297170"/>
+              <a:ext cx="444500" cy="339672"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="76" name="Rectangle 75">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3453DB5-F660-1E8C-8196-B292A9548594}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9237870" y="4313662"/>
+              <a:ext cx="2915478" cy="273721"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="TextBox 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C2A7E12-ADF0-79F7-4A27-1AB096152B8F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9241997" y="4449913"/>
+            <a:ext cx="508000" cy="224119"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Alien</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="TextBox 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{260E367F-CAFC-E58B-9920-169D7BF16506}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9918782" y="4452470"/>
+            <a:ext cx="463177" cy="209177"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Ape</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="24" name="TextBox 23">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DA325FF-271A-64C4-AEDB-3EE243E478D5}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10490224" y="4445001"/>
+            <a:ext cx="620059" cy="224116"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Zombie</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="25" name="TextBox 24">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1009377B-0A6D-97C3-8896-CEFB8CEFF67E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11218547" y="4441265"/>
+            <a:ext cx="612588" cy="231588"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Female</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="26" name="TextBox 25">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65184E0E-E175-8E1B-79FF-287F07F3E999}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11939402" y="4437529"/>
+            <a:ext cx="478118" cy="239059"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Male</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>289112</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>156471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>904688</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>40563</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="40" name="Group 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E83AF71E-583C-14CC-33FF-B9CCAAC7EB1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="289112" y="4156971"/>
+          <a:ext cx="615576" cy="1789092"/>
+          <a:chOff x="9657230" y="4922707"/>
+          <a:chExt cx="615576" cy="1751739"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="60" name="Group 59">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A83BDF5-2030-4BA6-A99C-AA29ED28D1F8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="9755589" y="4922707"/>
+            <a:ext cx="447049" cy="1751739"/>
+            <a:chOff x="359403" y="3916320"/>
+            <a:chExt cx="447049" cy="1721477"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="75" name="Rectangle 74">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B9B9AEB-2F64-6AE1-007E-388D8D283905}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="361156" y="3916320"/>
+              <a:ext cx="444500" cy="339851"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="73" name="Rectangle 72">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89A6A910-D7C9-564A-F257-17BFF99E8F70}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="359403" y="4256171"/>
+              <a:ext cx="444500" cy="345408"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="71" name="Rectangle 70">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB064605-AF85-F05E-4BF1-231BB3FCC5F7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="360364" y="4602204"/>
+              <a:ext cx="444500" cy="345407"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="69" name="Rectangle 68">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E681DB28-900B-8BB5-C0C0-6164B255F5FF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="361952" y="4944895"/>
+              <a:ext cx="444500" cy="345408"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="67" name="Rectangle 66">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1BE677F-7587-624C-C780-B802948DB094}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="359571" y="5292390"/>
+              <a:ext cx="444500" cy="345407"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="81" name="TextBox 80">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5CF68AC-94CB-4E17-8AE9-8866F48E94E3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9732913" y="6370948"/>
+            <a:ext cx="508000" cy="224119"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Alien</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="87" name="TextBox 86">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C42D819-3459-48E3-929A-9F9237B6FF79}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9785978" y="6002867"/>
+            <a:ext cx="463177" cy="209177"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Ape</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="88" name="TextBox 87">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D51471C-3C80-4B4B-AC9D-CB56F2012B3A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9657230" y="5655580"/>
+            <a:ext cx="615576" cy="206186"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Zombie</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="89" name="TextBox 88">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43E0FC6D-4D5D-4DD8-8465-6C6D4061D3FE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9658724" y="5314048"/>
+            <a:ext cx="612588" cy="231588"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Female</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="90" name="TextBox 89">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B95F0FFC-0BF8-4EB5-AF3B-AAF056E73163}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9725959" y="4942787"/>
+            <a:ext cx="478118" cy="239059"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Male</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -8827,6 +8825,1242 @@
     </cdr:sp>
   </cdr:relSizeAnchor>
 </c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>11190</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>15115</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Group 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04205B9E-D5E9-4D92-A9D6-2B8D33C68139}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3048000" y="2762250"/>
+          <a:ext cx="3059190" cy="383415"/>
+          <a:chOff x="9163969" y="4272977"/>
+          <a:chExt cx="3057219" cy="374320"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="3" name="Group 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E227E6E8-3E72-C0A6-4BFB-A6D302D06A67}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="11772790" y="4274122"/>
+            <a:ext cx="448398" cy="336133"/>
+            <a:chOff x="361156" y="3924372"/>
+            <a:chExt cx="444500" cy="341673"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="17" name="Picture 16">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{655B124F-CF3C-E371-A8B9-F4AF1214D884}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="497052" y="3982672"/>
+              <a:ext cx="179519" cy="256329"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="18" name="Rectangle 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B571AA0-0C78-43A6-9409-EDDAAD5AEB87}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="361156" y="3924372"/>
+              <a:ext cx="444500" cy="341673"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="4" name="Group 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01E11ABA-B103-D68A-3D2A-102655E9B4AA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="11136036" y="4305586"/>
+            <a:ext cx="444500" cy="341711"/>
+            <a:chOff x="362745" y="4256768"/>
+            <a:chExt cx="444500" cy="345169"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="15" name="Picture 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66B94A96-E2DB-4883-53A4-2D0F17D80D44}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="508000" y="4288518"/>
+              <a:ext cx="162903" cy="254268"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="16" name="Rectangle 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C3F57B0-2D2A-F9DF-BEBE-065C0F53ECE5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="362745" y="4256768"/>
+              <a:ext cx="444500" cy="345169"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="5" name="Group 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9301610-7DBF-4928-4D7D-94212790A4C8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="10479586" y="4290958"/>
+            <a:ext cx="444500" cy="341710"/>
+            <a:chOff x="360364" y="4605904"/>
+            <a:chExt cx="444500" cy="345169"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="13" name="Picture 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54193631-05BF-C347-91C0-5D1C5DF5E19B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+              <a:duotone>
+                <a:prstClr val="black"/>
+                <a:srgbClr val="7DA269">
+                  <a:tint val="45000"/>
+                  <a:satMod val="400000"/>
+                </a:srgbClr>
+              </a:duotone>
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="465932" y="4636862"/>
+              <a:ext cx="252000" cy="251546"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="Rectangle 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3546AAAA-4406-6ECD-0ACD-1D24C7E32F5A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="360364" y="4605904"/>
+              <a:ext cx="444500" cy="345169"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="6" name="Group 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA61E829-A048-66F6-8824-B772640C9D57}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="9808820" y="4272977"/>
+            <a:ext cx="444500" cy="341711"/>
+            <a:chOff x="361952" y="4955041"/>
+            <a:chExt cx="444500" cy="345168"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="11" name="Picture 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E141597-6093-62E1-568F-1B3F48F66C79}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+              <a:duotone>
+                <a:prstClr val="black"/>
+                <a:srgbClr val="E8D8CA">
+                  <a:tint val="45000"/>
+                  <a:satMod val="400000"/>
+                </a:srgbClr>
+              </a:duotone>
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="487362" y="5007428"/>
+              <a:ext cx="216314" cy="253133"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="Rectangle 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F70677FB-2938-5DAD-E953-A0A58D968FCD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="361952" y="4955041"/>
+              <a:ext cx="444500" cy="345168"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="7" name="Group 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91AB9AEA-51D6-9F8A-75BD-6E2DF23CB624}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="9163969" y="4297170"/>
+            <a:ext cx="444500" cy="339672"/>
+            <a:chOff x="359571" y="5292270"/>
+            <a:chExt cx="444500" cy="345169"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="9" name="Picture 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A22710B-E85B-40D3-D201-DF111FB2D3DF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+              <a:duotone>
+                <a:prstClr val="black"/>
+                <a:srgbClr val="C8FBFB">
+                  <a:tint val="45000"/>
+                  <a:satMod val="400000"/>
+                </a:srgbClr>
+              </a:duotone>
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="488950" y="5332753"/>
+              <a:ext cx="234354" cy="253134"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="Rectangle 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2D1BF18-8E0C-52BD-37F0-52EE3B99B349}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="359571" y="5292270"/>
+              <a:ext cx="444500" cy="345169"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Rectangle 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{486E0559-CB76-687F-20C6-E41F40D21FEE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9237870" y="4313662"/>
+            <a:ext cx="2915478" cy="273721"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>447049</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>94389</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="19" name="Group 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{686D6B4D-3BF3-46DA-A924-6C6028119273}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1828800" y="1657350"/>
+          <a:ext cx="447049" cy="1751739"/>
+          <a:chOff x="359403" y="3916320"/>
+          <a:chExt cx="447049" cy="1721477"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="20" name="Group 19">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91FF4EC0-4CC1-AA81-6A20-B65D39098742}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="361156" y="3916320"/>
+            <a:ext cx="444500" cy="339851"/>
+            <a:chOff x="361156" y="3924372"/>
+            <a:chExt cx="444500" cy="341673"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="33" name="Picture 32">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29C10864-019F-DE97-BAFD-CD3BDCE1073F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="497052" y="3982672"/>
+              <a:ext cx="179519" cy="256329"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="34" name="Rectangle 33">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5C6740F-0A6A-53C8-42E7-52A324AE890B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="361156" y="3924372"/>
+              <a:ext cx="444500" cy="341673"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="21" name="Group 20">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954CC397-A557-610A-12AF-D27D69B1C3EF}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="359403" y="4256171"/>
+            <a:ext cx="444500" cy="345408"/>
+            <a:chOff x="362745" y="4256768"/>
+            <a:chExt cx="444500" cy="345169"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="31" name="Picture 30">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AFB257B-196C-1352-DED1-355A27B3FA41}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="508000" y="4288518"/>
+              <a:ext cx="162903" cy="254268"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="32" name="Rectangle 31">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DE0A572-693F-0975-E082-E991101E748E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="362745" y="4256768"/>
+              <a:ext cx="444500" cy="345169"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="22" name="Group 21">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CF459D2-EBA2-E8ED-FD29-E5051D2F2332}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="360364" y="4602204"/>
+            <a:ext cx="444500" cy="345407"/>
+            <a:chOff x="360364" y="4605904"/>
+            <a:chExt cx="444500" cy="345169"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="29" name="Picture 28">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{410543D3-5FF7-E791-C6BE-9070CC32E682}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+              <a:duotone>
+                <a:prstClr val="black"/>
+                <a:srgbClr val="7DA269">
+                  <a:tint val="45000"/>
+                  <a:satMod val="400000"/>
+                </a:srgbClr>
+              </a:duotone>
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="465932" y="4636862"/>
+              <a:ext cx="252000" cy="251546"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="30" name="Rectangle 29">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE57EF5-C91E-48FF-27DD-45E145F7F71F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="360364" y="4605904"/>
+              <a:ext cx="444500" cy="345169"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="23" name="Group 22">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{188F0481-745F-AD87-A428-FA2F4B72D1D1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="361952" y="4944895"/>
+            <a:ext cx="444500" cy="345408"/>
+            <a:chOff x="361952" y="4955041"/>
+            <a:chExt cx="444500" cy="345168"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="27" name="Picture 26">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{662B568A-D1B0-E77B-6914-1047DCA573AA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+              <a:duotone>
+                <a:prstClr val="black"/>
+                <a:srgbClr val="E8D8CA">
+                  <a:tint val="45000"/>
+                  <a:satMod val="400000"/>
+                </a:srgbClr>
+              </a:duotone>
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="487362" y="5007428"/>
+              <a:ext cx="216314" cy="253133"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="28" name="Rectangle 27">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B46BBE6-D3A2-C290-C03C-1CF160558FCF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="361952" y="4955041"/>
+              <a:ext cx="444500" cy="345168"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="24" name="Group 23">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC64B737-3AC8-FB11-52A6-754AE151B057}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="359571" y="5292390"/>
+            <a:ext cx="444500" cy="345407"/>
+            <a:chOff x="359571" y="5292270"/>
+            <a:chExt cx="444500" cy="345169"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="25" name="Picture 24">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81F96B50-F22A-D6B7-77A2-DA0A600ACAC3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+              <a:duotone>
+                <a:prstClr val="black"/>
+                <a:srgbClr val="C8FBFB">
+                  <a:tint val="45000"/>
+                  <a:satMod val="400000"/>
+                </a:srgbClr>
+              </a:duotone>
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="488950" y="5332753"/>
+              <a:ext cx="234354" cy="253134"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="26" name="Rectangle 25">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D22ACBE-B973-6D25-3AC8-14258D9709A2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="359571" y="5292270"/>
+              <a:ext cx="444500" cy="345169"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9183,15 +10417,15 @@
         <v>343</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -9203,8 +10437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6946B6DC-972A-4A33-9276-1E5BC691C458}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection sqref="A1:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9213,7 +10447,7 @@
     <col min="2" max="2" width="50.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="56" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
         <v>341</v>
       </c>
@@ -9227,10 +10461,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84654BBE-EADC-4B95-9774-3D220BD1BEE5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -11400,7 +12649,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA57CDC8-14C7-4CD1-A31D-3A27E9F197C3}">
   <dimension ref="A1:E101"/>
   <sheetViews>
@@ -11433,7 +12682,7 @@
         <v>100</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
changed the data viz - sorted bar charts, removed redundant worksheet
</commit_message>
<xml_diff>
--- a/Analysis_Worksheets/cryptopunks.xlsx
+++ b/Analysis_Worksheets/cryptopunks.xlsx
@@ -8,19 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Analysis_of_Cryptopunks_Top_60\Analysis_Worksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F35B62-2772-4E88-9E71-26A56EA8ACE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83570B7B-0EBA-4A20-8944-A836DA72CEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_xltb_storage_" sheetId="5" state="veryHidden" r:id="rId1"/>
     <sheet name="Data viz" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
-    <sheet name="cryptopunks" sheetId="1" r:id="rId4"/>
-    <sheet name="attributes" sheetId="3" r:id="rId5"/>
+    <sheet name="cryptopunks" sheetId="1" r:id="rId3"/>
+    <sheet name="attributes" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">attributes!$B$1:$B$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">attributes!$B$1:$B$101</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,30 +37,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="348">
   <si>
     <t>#5822</t>
   </si>
@@ -2421,10 +2398,10 @@
                   <c:v>Zombie</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Female</c:v>
+                  <c:v>Male</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Male</c:v>
+                  <c:v>Female</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2445,10 +2422,10 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2478,12 +2455,42 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="1332142416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -2499,7 +2506,7 @@
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1332138256"/>
@@ -2649,9 +2656,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="3.6852379444972036E-2"/>
-          <c:y val="0.25300667287399126"/>
+          <c:y val="0.28310851862473918"/>
           <c:w val="0.9262952411100559"/>
-          <c:h val="0.62341364059590321"/>
+          <c:h val="0.59331212782717035"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2746,22 +2753,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>6 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0 Attributes</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1 Attributes</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2 Attributes</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>3 Attributes</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>4 Attributes</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6 Attributes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2773,19 +2780,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2</c:v>
@@ -2818,12 +2825,45 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="1187322848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -3073,10 +3113,10 @@
                   <c:v>Zombie</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Female</c:v>
+                  <c:v>Male</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Male</c:v>
+                  <c:v>Female</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3097,10 +3137,10 @@
                   <c:v>0.23863636363636365</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8229166666666667E-3</c:v>
+                  <c:v>2.3182646133465806E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3182646133465806E-3</c:v>
+                  <c:v>1.8229166666666667E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3127,14 +3167,47 @@
       <c:catAx>
         <c:axId val="1847241631"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="1847243711"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -3148,7 +3221,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -3424,22 +3497,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>6 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0 Attributes</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1 Attributes</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2 Attributes</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>3 Attributes</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>4 Attributes</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6 Attributes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3451,22 +3524,22 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0.18181818181818182</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.125</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2.7027027027027029E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>5.3370786516853935E-3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4.2212841590757609E-3</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1.4084507042253522E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.18181818181818182</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3493,14 +3566,47 @@
       <c:catAx>
         <c:axId val="73912831"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="73916575"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -3514,7 +3620,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -5849,8 +5955,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="219364" y="2300942"/>
-          <a:ext cx="1604818" cy="1143000"/>
+          <a:off x="219364" y="2282799"/>
+          <a:ext cx="1604818" cy="1088572"/>
           <a:chOff x="6021294" y="11586883"/>
           <a:chExt cx="1837850" cy="1234004"/>
         </a:xfrm>
@@ -6009,8 +6115,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2401511" y="2293816"/>
-          <a:ext cx="1605600" cy="1143436"/>
+          <a:off x="2401511" y="2275673"/>
+          <a:ext cx="1605600" cy="1089008"/>
           <a:chOff x="6021297" y="11586883"/>
           <a:chExt cx="1763059" cy="1135530"/>
         </a:xfrm>
@@ -6383,8 +6489,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4584440" y="2305015"/>
-          <a:ext cx="1604819" cy="1143436"/>
+          <a:off x="4584440" y="2286872"/>
+          <a:ext cx="1604819" cy="1089008"/>
           <a:chOff x="3635460" y="2163074"/>
           <a:chExt cx="1604819" cy="1121024"/>
         </a:xfrm>
@@ -6581,8 +6687,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="23091" y="682625"/>
-          <a:ext cx="8595167" cy="1397000"/>
+          <a:off x="23091" y="680357"/>
+          <a:ext cx="8597435" cy="1397000"/>
           <a:chOff x="23091" y="679824"/>
           <a:chExt cx="8597968" cy="1397000"/>
         </a:xfrm>
@@ -6674,8 +6780,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="2196353" y="922249"/>
-            <a:ext cx="6338047" cy="885633"/>
+            <a:off x="2150993" y="849678"/>
+            <a:ext cx="6338047" cy="1072932"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -6712,7 +6818,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1200" baseline="0"/>
-              <a:t> the NFT Craze of 2021. There are 10,000 CryptoPunks in general and are classified based on punk types: Ape, Alien, Female, Male and Zombie; Attributes they possess and Attribute Counts . This project was carried out to analyse if the price a punk is sold at depends on rarity of a punk type or attribute count.</a:t>
+              <a:t> the NFT Craze of 2021. There are 10,000 CryptoPunks in general and are classified based on punk types: Ape, Alien, Female, Male and Zombie; Attributes they possess and Attribute Counts . This project was carried out to analyse the trend of the percentage of the punk types and attribute counts according to their rarity in the top sales.</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1200"/>
           </a:p>
@@ -6803,8 +6909,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6766588" y="2295778"/>
-          <a:ext cx="1604819" cy="1144765"/>
+          <a:off x="6766588" y="2277635"/>
+          <a:ext cx="1604819" cy="1090337"/>
           <a:chOff x="3635460" y="2163074"/>
           <a:chExt cx="1604819" cy="1122368"/>
         </a:xfrm>
@@ -7082,353 +7188,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>275937</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>9992</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1080177</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>127880</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="TextBox 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB8B4724-B7E8-35F9-22AD-24457CD001CD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="275937" y="7248992"/>
-          <a:ext cx="804240" cy="1832388"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="875">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>6 Attributes</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="875">
-            <a:solidFill>
-              <a:schemeClr val="bg2">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="875">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>4 </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="875">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Attributes</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="875">
-            <a:solidFill>
-              <a:schemeClr val="bg2">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="875">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>3 Attributes</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="875">
-            <a:solidFill>
-              <a:schemeClr val="bg2">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="875">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>2 Attributes</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="875">
-            <a:solidFill>
-              <a:schemeClr val="bg2">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="875">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>1 Attributes</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="875">
-            <a:solidFill>
-              <a:schemeClr val="bg2">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="875">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>0 Attributes</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="875">
-            <a:solidFill>
-              <a:schemeClr val="bg2">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4660900</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>8324850</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="TextBox 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E47103E2-E928-727D-14F7-365B5535955A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4660900" y="8832850"/>
-          <a:ext cx="3663950" cy="228600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="900">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>0 </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="900">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Attributes 1 Attributes 2 Attributes 3 Attributes 4 Attributes 6</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="900">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Attributes</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="900">
-            <a:solidFill>
-              <a:schemeClr val="bg2">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
@@ -7488,1259 +7247,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4956969</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>169755</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>8032752</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>179640</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="28" name="Group 27">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01C95BEB-78D5-4BB7-1D3A-7BEDD9520C5A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="4956969" y="5694255"/>
-          <a:ext cx="3075783" cy="390885"/>
-          <a:chOff x="9241810" y="4375696"/>
-          <a:chExt cx="3175710" cy="383415"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="77" name="Group 76">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FD7AD55-3018-A18B-73A7-069575407410}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="9241810" y="4375696"/>
-            <a:ext cx="3059190" cy="383415"/>
-            <a:chOff x="9163969" y="4272977"/>
-            <a:chExt cx="3057219" cy="374320"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="30" name="Rectangle 29">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F53AD360-D2C3-2068-BFEE-B3D7449B92B7}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="11772790" y="4274122"/>
-              <a:ext cx="448398" cy="336133"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="31" name="Rectangle 30">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{362ABB6C-2E52-4554-A325-56B8629D6FAD}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="11136036" y="4305586"/>
-              <a:ext cx="444500" cy="341711"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="32" name="Rectangle 31">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FC6C50A-0BDD-45FB-B3A7-B0B7873489AC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="10479586" y="4290958"/>
-              <a:ext cx="444500" cy="341710"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="33" name="Rectangle 32">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EAC67AD-7CA9-41A3-B3A1-330355D347E3}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="9808820" y="4272977"/>
-              <a:ext cx="444500" cy="341711"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="34" name="Rectangle 33">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A725F3E-56B5-4425-987A-38AAC35FE5AF}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="9163969" y="4297170"/>
-              <a:ext cx="444500" cy="339672"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="76" name="Rectangle 75">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3453DB5-F660-1E8C-8196-B292A9548594}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="9237870" y="4313662"/>
-              <a:ext cx="2915478" cy="273721"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="7" name="TextBox 6">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C2A7E12-ADF0-79F7-4A27-1AB096152B8F}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9241997" y="4449913"/>
-            <a:ext cx="508000" cy="224119"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="900">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Alien</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="TextBox 7">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{260E367F-CAFC-E58B-9920-169D7BF16506}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9918782" y="4452470"/>
-            <a:ext cx="463177" cy="209177"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="900">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Ape</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="24" name="TextBox 23">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DA325FF-271A-64C4-AEDB-3EE243E478D5}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="10490224" y="4445001"/>
-            <a:ext cx="620059" cy="224116"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="900">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Zombie</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="25" name="TextBox 24">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1009377B-0A6D-97C3-8896-CEFB8CEFF67E}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="11218547" y="4441265"/>
-            <a:ext cx="612588" cy="231588"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="900">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Female</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:endParaRPr lang="en-US" sz="900">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="26" name="TextBox 25">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65184E0E-E175-8E1B-79FF-287F07F3E999}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="11939402" y="4437529"/>
-            <a:ext cx="478118" cy="239059"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="900">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Male</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>289112</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>156471</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>904688</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>40563</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="40" name="Group 39">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E83AF71E-583C-14CC-33FF-B9CCAAC7EB1C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="289112" y="4156971"/>
-          <a:ext cx="615576" cy="1789092"/>
-          <a:chOff x="9657230" y="4922707"/>
-          <a:chExt cx="615576" cy="1751739"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="60" name="Group 59">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A83BDF5-2030-4BA6-A99C-AA29ED28D1F8}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="9755589" y="4922707"/>
-            <a:ext cx="447049" cy="1751739"/>
-            <a:chOff x="359403" y="3916320"/>
-            <a:chExt cx="447049" cy="1721477"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="75" name="Rectangle 74">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B9B9AEB-2F64-6AE1-007E-388D8D283905}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="361156" y="3916320"/>
-              <a:ext cx="444500" cy="339851"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="73" name="Rectangle 72">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89A6A910-D7C9-564A-F257-17BFF99E8F70}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="359403" y="4256171"/>
-              <a:ext cx="444500" cy="345408"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="71" name="Rectangle 70">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB064605-AF85-F05E-4BF1-231BB3FCC5F7}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="360364" y="4602204"/>
-              <a:ext cx="444500" cy="345407"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="69" name="Rectangle 68">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E681DB28-900B-8BB5-C0C0-6164B255F5FF}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="361952" y="4944895"/>
-              <a:ext cx="444500" cy="345408"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="67" name="Rectangle 66">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1BE677F-7587-624C-C780-B802948DB094}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="359571" y="5292390"/>
-              <a:ext cx="444500" cy="345407"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="81" name="TextBox 80">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5CF68AC-94CB-4E17-8AE9-8866F48E94E3}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9732913" y="6370948"/>
-            <a:ext cx="508000" cy="224119"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="900">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Alien</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="87" name="TextBox 86">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C42D819-3459-48E3-929A-9F9237B6FF79}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9785978" y="6002867"/>
-            <a:ext cx="463177" cy="209177"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="900">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Ape</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="88" name="TextBox 87">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D51471C-3C80-4B4B-AC9D-CB56F2012B3A}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9657230" y="5655580"/>
-            <a:ext cx="615576" cy="206186"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="900">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Zombie</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="89" name="TextBox 88">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43E0FC6D-4D5D-4DD8-8465-6C6D4061D3FE}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9658724" y="5314048"/>
-            <a:ext cx="612588" cy="231588"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="900">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Female</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:endParaRPr lang="en-US" sz="900">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="90" name="TextBox 89">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B95F0FFC-0BF8-4EB5-AF3B-AAF056E73163}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9725959" y="4942787"/>
-            <a:ext cx="478118" cy="239059"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="900">
-                <a:solidFill>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Male</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -8825,1242 +7331,6 @@
     </cdr:sp>
   </cdr:relSizeAnchor>
 </c:userShapes>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>11190</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>15115</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="Group 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04205B9E-D5E9-4D92-A9D6-2B8D33C68139}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="3048000" y="2762250"/>
-          <a:ext cx="3059190" cy="383415"/>
-          <a:chOff x="9163969" y="4272977"/>
-          <a:chExt cx="3057219" cy="374320"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="3" name="Group 2">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E227E6E8-3E72-C0A6-4BFB-A6D302D06A67}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="11772790" y="4274122"/>
-            <a:ext cx="448398" cy="336133"/>
-            <a:chOff x="361156" y="3924372"/>
-            <a:chExt cx="444500" cy="341673"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="17" name="Picture 16">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{655B124F-CF3C-E371-A8B9-F4AF1214D884}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="497052" y="3982672"/>
-              <a:ext cx="179519" cy="256329"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="18" name="Rectangle 17">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B571AA0-0C78-43A6-9409-EDDAAD5AEB87}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="361156" y="3924372"/>
-              <a:ext cx="444500" cy="341673"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="4" name="Group 3">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01E11ABA-B103-D68A-3D2A-102655E9B4AA}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="11136036" y="4305586"/>
-            <a:ext cx="444500" cy="341711"/>
-            <a:chOff x="362745" y="4256768"/>
-            <a:chExt cx="444500" cy="345169"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="15" name="Picture 14">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66B94A96-E2DB-4883-53A4-2D0F17D80D44}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="508000" y="4288518"/>
-              <a:ext cx="162903" cy="254268"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="16" name="Rectangle 15">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C3F57B0-2D2A-F9DF-BEBE-065C0F53ECE5}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="362745" y="4256768"/>
-              <a:ext cx="444500" cy="345169"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="5" name="Group 4">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9301610-7DBF-4928-4D7D-94212790A4C8}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="10479586" y="4290958"/>
-            <a:ext cx="444500" cy="341710"/>
-            <a:chOff x="360364" y="4605904"/>
-            <a:chExt cx="444500" cy="345169"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="13" name="Picture 12">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54193631-05BF-C347-91C0-5D1C5DF5E19B}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-              <a:duotone>
-                <a:prstClr val="black"/>
-                <a:srgbClr val="7DA269">
-                  <a:tint val="45000"/>
-                  <a:satMod val="400000"/>
-                </a:srgbClr>
-              </a:duotone>
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="465932" y="4636862"/>
-              <a:ext cx="252000" cy="251546"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="Rectangle 13">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3546AAAA-4406-6ECD-0ACD-1D24C7E32F5A}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="360364" y="4605904"/>
-              <a:ext cx="444500" cy="345169"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="6" name="Group 5">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA61E829-A048-66F6-8824-B772640C9D57}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="9808820" y="4272977"/>
-            <a:ext cx="444500" cy="341711"/>
-            <a:chOff x="361952" y="4955041"/>
-            <a:chExt cx="444500" cy="345168"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="11" name="Picture 10">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E141597-6093-62E1-568F-1B3F48F66C79}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-              <a:duotone>
-                <a:prstClr val="black"/>
-                <a:srgbClr val="E8D8CA">
-                  <a:tint val="45000"/>
-                  <a:satMod val="400000"/>
-                </a:srgbClr>
-              </a:duotone>
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="487362" y="5007428"/>
-              <a:ext cx="216314" cy="253133"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="12" name="Rectangle 11">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F70677FB-2938-5DAD-E953-A0A58D968FCD}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="361952" y="4955041"/>
-              <a:ext cx="444500" cy="345168"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="7" name="Group 6">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91AB9AEA-51D6-9F8A-75BD-6E2DF23CB624}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="9163969" y="4297170"/>
-            <a:ext cx="444500" cy="339672"/>
-            <a:chOff x="359571" y="5292270"/>
-            <a:chExt cx="444500" cy="345169"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="9" name="Picture 8">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A22710B-E85B-40D3-D201-DF111FB2D3DF}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-              <a:duotone>
-                <a:prstClr val="black"/>
-                <a:srgbClr val="C8FBFB">
-                  <a:tint val="45000"/>
-                  <a:satMod val="400000"/>
-                </a:srgbClr>
-              </a:duotone>
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="488950" y="5332753"/>
-              <a:ext cx="234354" cy="253134"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="10" name="Rectangle 9">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2D1BF18-8E0C-52BD-37F0-52EE3B99B349}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="359571" y="5292270"/>
-              <a:ext cx="444500" cy="345169"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="Rectangle 7">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{486E0559-CB76-687F-20C6-E41F40D21FEE}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9237870" y="4313662"/>
-            <a:ext cx="2915478" cy="273721"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>447049</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>94389</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="19" name="Group 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{686D6B4D-3BF3-46DA-A924-6C6028119273}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1828800" y="1657350"/>
-          <a:ext cx="447049" cy="1751739"/>
-          <a:chOff x="359403" y="3916320"/>
-          <a:chExt cx="447049" cy="1721477"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="20" name="Group 19">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91FF4EC0-4CC1-AA81-6A20-B65D39098742}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="361156" y="3916320"/>
-            <a:ext cx="444500" cy="339851"/>
-            <a:chOff x="361156" y="3924372"/>
-            <a:chExt cx="444500" cy="341673"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="33" name="Picture 32">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29C10864-019F-DE97-BAFD-CD3BDCE1073F}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="497052" y="3982672"/>
-              <a:ext cx="179519" cy="256329"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="34" name="Rectangle 33">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5C6740F-0A6A-53C8-42E7-52A324AE890B}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="361156" y="3924372"/>
-              <a:ext cx="444500" cy="341673"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="21" name="Group 20">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954CC397-A557-610A-12AF-D27D69B1C3EF}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="359403" y="4256171"/>
-            <a:ext cx="444500" cy="345408"/>
-            <a:chOff x="362745" y="4256768"/>
-            <a:chExt cx="444500" cy="345169"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="31" name="Picture 30">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AFB257B-196C-1352-DED1-355A27B3FA41}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="508000" y="4288518"/>
-              <a:ext cx="162903" cy="254268"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="32" name="Rectangle 31">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DE0A572-693F-0975-E082-E991101E748E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="362745" y="4256768"/>
-              <a:ext cx="444500" cy="345169"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="22" name="Group 21">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CF459D2-EBA2-E8ED-FD29-E5051D2F2332}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="360364" y="4602204"/>
-            <a:ext cx="444500" cy="345407"/>
-            <a:chOff x="360364" y="4605904"/>
-            <a:chExt cx="444500" cy="345169"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="29" name="Picture 28">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{410543D3-5FF7-E791-C6BE-9070CC32E682}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-              <a:duotone>
-                <a:prstClr val="black"/>
-                <a:srgbClr val="7DA269">
-                  <a:tint val="45000"/>
-                  <a:satMod val="400000"/>
-                </a:srgbClr>
-              </a:duotone>
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="465932" y="4636862"/>
-              <a:ext cx="252000" cy="251546"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="30" name="Rectangle 29">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE57EF5-C91E-48FF-27DD-45E145F7F71F}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="360364" y="4605904"/>
-              <a:ext cx="444500" cy="345169"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="23" name="Group 22">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{188F0481-745F-AD87-A428-FA2F4B72D1D1}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="361952" y="4944895"/>
-            <a:ext cx="444500" cy="345408"/>
-            <a:chOff x="361952" y="4955041"/>
-            <a:chExt cx="444500" cy="345168"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="27" name="Picture 26">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{662B568A-D1B0-E77B-6914-1047DCA573AA}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-              <a:duotone>
-                <a:prstClr val="black"/>
-                <a:srgbClr val="E8D8CA">
-                  <a:tint val="45000"/>
-                  <a:satMod val="400000"/>
-                </a:srgbClr>
-              </a:duotone>
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="487362" y="5007428"/>
-              <a:ext cx="216314" cy="253133"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="28" name="Rectangle 27">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B46BBE6-D3A2-C290-C03C-1CF160558FCF}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="361952" y="4955041"/>
-              <a:ext cx="444500" cy="345168"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="24" name="Group 23">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC64B737-3AC8-FB11-52A6-754AE151B057}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="359571" y="5292390"/>
-            <a:ext cx="444500" cy="345407"/>
-            <a:chOff x="359571" y="5292270"/>
-            <a:chExt cx="444500" cy="345169"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="25" name="Picture 24">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81F96B50-F22A-D6B7-77A2-DA0A600ACAC3}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-              <a:duotone>
-                <a:prstClr val="black"/>
-                <a:srgbClr val="C8FBFB">
-                  <a:tint val="45000"/>
-                  <a:satMod val="400000"/>
-                </a:srgbClr>
-              </a:duotone>
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="488950" y="5332753"/>
-              <a:ext cx="234354" cy="253134"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="26" name="Rectangle 25">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D22ACBE-B973-6D25-3AC8-14258D9709A2}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="359571" y="5292270"/>
-              <a:ext cx="444500" cy="345169"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10437,8 +7707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6946B6DC-972A-4A33-9276-1E5BC691C458}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection sqref="A1:A40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10461,26 +7731,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84654BBE-EADC-4B95-9774-3D220BD1BEE5}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12420,112 +9675,109 @@
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A64" s="13" t="str" cm="1">
-        <f t="array" ref="A64:A70">_xlfn._xlws.SORT(_xlfn.UNIQUE($I$2:$I$61))</f>
-        <v>0 Attributes</v>
+      <c r="A64" s="13" t="s">
+        <v>202</v>
       </c>
       <c r="B64" s="2">
         <f xml:space="preserve"> COUNTIF($I$2:$I$61, A64)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C64" s="2">
         <f>VLOOKUP(A64, attributes!$A$1:$E$101, 2, FALSE)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D64" s="11">
         <f>B64/C64</f>
-        <v>0.125</v>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="7" t="str">
-        <v>1 Attributes</v>
+      <c r="A65" s="7" t="s">
+        <v>196</v>
       </c>
       <c r="B65" s="2">
-        <f t="shared" ref="B65:B69" si="2" xml:space="preserve"> COUNTIF($I$2:$I$61, A65)</f>
-        <v>9</v>
+        <f xml:space="preserve"> COUNTIF($I$2:$I$61, A65)</f>
+        <v>1</v>
       </c>
       <c r="C65" s="2">
         <f>VLOOKUP(A65, attributes!$A$1:$E$101, 2, FALSE)</f>
-        <v>333</v>
+        <v>8</v>
       </c>
       <c r="D65" s="11">
-        <f t="shared" ref="D65:D69" si="3">B65/C65</f>
-        <v>2.7027027027027029E-2</v>
+        <f>B65/C65</f>
+        <v>0.125</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="13" t="str">
-        <v>2 Attributes</v>
+      <c r="A66" s="13" t="s">
+        <v>197</v>
       </c>
       <c r="B66" s="2">
-        <f t="shared" si="2"/>
-        <v>19</v>
+        <f xml:space="preserve"> COUNTIF($I$2:$I$61, A66)</f>
+        <v>9</v>
       </c>
       <c r="C66" s="2">
         <f>VLOOKUP(A66, attributes!$A$1:$E$101, 2, FALSE)</f>
-        <v>3560</v>
+        <v>333</v>
       </c>
       <c r="D66" s="11">
-        <f t="shared" si="3"/>
-        <v>5.3370786516853935E-3</v>
+        <f>B66/C66</f>
+        <v>2.7027027027027029E-2</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="13" t="str">
-        <v>3 Attributes</v>
+      <c r="A67" s="13" t="s">
+        <v>198</v>
       </c>
       <c r="B67" s="2">
-        <f t="shared" si="2"/>
+        <f xml:space="preserve"> COUNTIF($I$2:$I$61, A67)</f>
         <v>19</v>
       </c>
       <c r="C67" s="2">
         <f>VLOOKUP(A67, attributes!$A$1:$E$101, 2, FALSE)</f>
-        <v>4501</v>
+        <v>3560</v>
       </c>
       <c r="D67" s="11">
-        <f t="shared" si="3"/>
-        <v>4.2212841590757609E-3</v>
+        <f>B67/C67</f>
+        <v>5.3370786516853935E-3</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" s="13" t="str">
-        <v>4 Attributes</v>
+      <c r="A68" s="13" t="s">
+        <v>199</v>
       </c>
       <c r="B68" s="2">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f xml:space="preserve"> COUNTIF($I$2:$I$61, A68)</f>
+        <v>19</v>
       </c>
       <c r="C68" s="2">
         <f>VLOOKUP(A68, attributes!$A$1:$E$101, 2, FALSE)</f>
-        <v>1420</v>
+        <v>4501</v>
       </c>
       <c r="D68" s="11">
-        <f t="shared" si="3"/>
-        <v>1.4084507042253522E-3</v>
+        <f>B68/C68</f>
+        <v>4.2212841590757609E-3</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="14" t="str">
-        <v>6 Attributes</v>
+      <c r="A69" s="14" t="s">
+        <v>200</v>
       </c>
       <c r="B69" s="4">
-        <f t="shared" si="2"/>
+        <f xml:space="preserve"> COUNTIF($I$2:$I$61, A69)</f>
         <v>2</v>
       </c>
       <c r="C69" s="4">
         <f>VLOOKUP(A69, attributes!$A$1:$E$101, 2, FALSE)</f>
-        <v>11</v>
+        <v>1420</v>
       </c>
       <c r="D69" s="12">
-        <f t="shared" si="3"/>
-        <v>0.18181818181818182</v>
+        <f>B69/C69</f>
+        <v>1.4084507042253522E-3</v>
       </c>
     </row>
     <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="15">
-        <v>0</v>
-      </c>
+      <c r="A70" s="15"/>
     </row>
     <row r="73" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
@@ -12543,9 +9795,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75" s="7" t="str" cm="1">
-        <f t="array" ref="A75:A79">_xlfn.UNIQUE(K2:K53)</f>
-        <v>Alien</v>
+      <c r="A75" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="B75" s="2">
         <f>COUNTIF($K$2:$K$61, A75)</f>
@@ -12561,11 +9812,11 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" s="7" t="str">
-        <v>Ape</v>
+      <c r="A76" t="s">
+        <v>102</v>
       </c>
       <c r="B76" s="2">
-        <f t="shared" ref="B76:B79" si="4">COUNTIF($K$2:$K$61, A76)</f>
+        <f>COUNTIF($K$2:$K$61, A76)</f>
         <v>6</v>
       </c>
       <c r="C76" s="2">
@@ -12573,16 +9824,16 @@
         <v>24</v>
       </c>
       <c r="D76" s="11">
-        <f t="shared" ref="D76:D79" si="5">B76/C76</f>
+        <f>B76/C76</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77" s="7" t="str">
-        <v>Zombie</v>
+      <c r="A77" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B77" s="2">
-        <f t="shared" si="4"/>
+        <f>COUNTIF($K$2:$K$61, A77)</f>
         <v>21</v>
       </c>
       <c r="C77" s="2">
@@ -12590,42 +9841,42 @@
         <v>88</v>
       </c>
       <c r="D77" s="11">
-        <f t="shared" si="5"/>
+        <f>B77/C77</f>
         <v>0.23863636363636365</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A78" s="7" t="str">
-        <v>Female</v>
+      <c r="A78" s="7" t="s">
+        <v>107</v>
       </c>
       <c r="B78" s="2">
-        <f t="shared" si="4"/>
-        <v>7</v>
+        <f t="shared" ref="B76:B79" si="2">COUNTIF($K$2:$K$61, A78)</f>
+        <v>14</v>
       </c>
       <c r="C78" s="2">
         <f>VLOOKUP(A78, attributes!$A$1:$E$101, 2, FALSE)</f>
-        <v>3840</v>
+        <v>6039</v>
       </c>
       <c r="D78" s="11">
-        <f t="shared" si="5"/>
-        <v>1.8229166666666667E-3</v>
+        <f>B78/C78</f>
+        <v>2.3182646133465806E-3</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="8" t="str">
-        <v>Male</v>
+      <c r="A79" s="8" t="s">
+        <v>106</v>
       </c>
       <c r="B79" s="4">
-        <f t="shared" si="4"/>
-        <v>14</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="C79" s="4">
         <f>VLOOKUP(A79, attributes!$A$1:$E$101, 2, FALSE)</f>
-        <v>6039</v>
+        <v>3840</v>
       </c>
       <c r="D79" s="12">
-        <f t="shared" si="5"/>
-        <v>2.3182646133465806E-3</v>
+        <f>B79/C79</f>
+        <v>1.8229166666666667E-3</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -12649,7 +9900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA57CDC8-14C7-4CD1-A31D-3A27E9F197C3}">
   <dimension ref="A1:E101"/>
   <sheetViews>

</xml_diff>

<commit_message>
changed the data viz to a more appropriate group clustered column chart
</commit_message>
<xml_diff>
--- a/Analysis_Worksheets/cryptopunks.xlsx
+++ b/Analysis_Worksheets/cryptopunks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Analysis_of_Cryptopunks_Top_60\Analysis_Worksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83570B7B-0EBA-4A20-8944-A836DA72CEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C77206-52D8-4C34-BDB2-A0BAEC55CCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="350">
   <si>
     <t>#5822</t>
   </si>
@@ -1099,6 +1099,12 @@
   </si>
   <si>
     <t>C:\Analysis_of_Cryptopunks_Top_60\data-viz.png</t>
+  </si>
+  <si>
+    <t>Percentage of attribute count not in top sales</t>
+  </si>
+  <si>
+    <t>Percentage of punk type not in top sales</t>
   </si>
 </sst>
 </file>
@@ -1733,9 +1739,7 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1748,9 +1752,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1802,7 +1804,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1814,13 +1816,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="16" fillId="0" borderId="16" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="18" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1831,6 +1829,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="21" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1878,16 +1885,6 @@
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -2194,12 +2191,23 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF638596"/>
+      <color rgb="FFF496D7"/>
       <color rgb="FFEA34B0"/>
-      <color rgb="FF638596"/>
       <color rgb="FFDBB180"/>
       <color rgb="FFE8D8CA"/>
       <color rgb="FF856F56"/>
@@ -2955,7 +2963,7 @@
             <a:pPr>
               <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2963,13 +2971,24 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="1">
+              <a:rPr lang="en-US" b="1" baseline="0">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Percentage of Punks in Top 60 By Type</a:t>
+              <a:t>Percentage of Punks in Top 60 by </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Attribute Count </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2988,7 +3007,7 @@
           <a:pPr>
             <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -3001,412 +3020,9 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.15589925515577902"/>
-          <c:y val="0.18499247137591204"/>
-          <c:w val="0.79401035904643302"/>
-          <c:h val="0.68430558751937143"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>cryptopunks!$D$74</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Percentage of punk type in top sales</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="EA34B0"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>cryptopunks!$A$75:$A$79</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Alien</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ape</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Zombie</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Male</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Female</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>cryptopunks!$D$75:$D$79</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.44444444444444442</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.23863636363636365</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.3182646133465806E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.8229166666666667E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D8D4-447D-9802-E5FC965479C8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="outEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="1847241631"/>
-        <c:axId val="1847243711"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1847241631"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1847243711"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1847243711"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="t"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1847241631"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
-      <a:round/>
-    </a:ln>
-    <a:effectLst>
-      <a:outerShdw blurRad="50800" dist="38100" algn="l" rotWithShape="0">
-        <a:srgbClr val="638596">
-          <a:alpha val="80000"/>
-        </a:srgbClr>
-      </a:outerShdw>
-    </a:effectLst>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:userShapes r:id="rId3"/>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" b="1">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Percentage of Punks</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>in Top 60 By </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>A</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>ttribute Count </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.2071233164983165"/>
-          <c:y val="0.26717292803522646"/>
-          <c:w val="0.74610690235690236"/>
-          <c:h val="0.64417301396470084"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="bar"/>
+        <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -3434,6 +3050,138 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1111111111111117E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-4F9B-4AF5-82B9-CC9D7C62F21A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.9444444444444445E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-4F9B-4AF5-82B9-CC9D7C62F21A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.3333333333333332E-3"/>
+                  <c:y val="8.4875562720133283E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-4F9B-4AF5-82B9-CC9D7C62F21A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5555555555555558E-3"/>
+                  <c:y val="-8.4875562720133283E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-4F9B-4AF5-82B9-CC9D7C62F21A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1111111111111212E-2"/>
+                  <c:y val="8.4875562720133283E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-4F9B-4AF5-82B9-CC9D7C62F21A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.3333333333333332E-3"/>
+                  <c:y val="-8.4875562720133283E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-4F9B-4AF5-82B9-CC9D7C62F21A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -3546,7 +3294,496 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1AA4-4550-94F3-2D90FCD275B8}"/>
+              <c16:uniqueId val="{00000006-4F9B-4AF5-82B9-CC9D7C62F21A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cryptopunks!$E$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>cryptopunks!$A$64:$A$69</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4 Attributes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cryptopunks!$E$64:$E$69</c:f>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-4F9B-4AF5-82B9-CC9D7C62F21A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cryptopunks!$F$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>cryptopunks!$A$64:$A$69</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4 Attributes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cryptopunks!$F$64:$F$69</c:f>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-4F9B-4AF5-82B9-CC9D7C62F21A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cryptopunks!$G$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>cryptopunks!$A$64:$A$69</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4 Attributes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cryptopunks!$G$64:$G$69</c:f>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-4F9B-4AF5-82B9-CC9D7C62F21A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cryptopunks!$H$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percentage of attribute count not in top sales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F496D7"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>cryptopunks!$A$64:$A$69</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Attributes</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4 Attributes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cryptopunks!$H$64:$H$69</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.81818181818181812</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97297297297297303</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99466292134831458</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99577871584092426</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99859154929577465</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-4F9B-4AF5-82B9-CC9D7C62F21A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3559,17 +3796,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="73912831"/>
-        <c:axId val="73916575"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1215215040"/>
+        <c:axId val="662734240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="73912831"/>
+        <c:axId val="1215215040"/>
         <c:scaling>
-          <c:orientation val="maxMin"/>
+          <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3607,26 +3845,27 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73916575"/>
+        <c:crossAx val="662734240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73916575"/>
+        <c:axId val="662734240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
-        <c:axPos val="t"/>
+        <c:axPos val="r"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73912831"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="1215215040"/>
+        <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -3637,13 +3876,995 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst>
+      <a:outerShdw blurRad="50800" dist="38100" algn="l" rotWithShape="0">
+        <a:srgbClr val="638596">
+          <a:alpha val="80000"/>
+        </a:srgbClr>
+      </a:outerShdw>
+    </a:effectLst>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Percentage of Punks in Top 60 by </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Type</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cryptopunks!$D$74</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percentage of punk type in top sales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="EA34B0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.3888888888888888E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-0415-4505-9CF8-5F1822558C11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1111111111111112E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-0415-4505-9CF8-5F1822558C11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.3888888888888888E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-0415-4505-9CF8-5F1822558C11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.3333333333333332E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-0415-4505-9CF8-5F1822558C11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>cryptopunks!$A$75:$A$79</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Alien</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ape</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Zombie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Male</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Female</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cryptopunks!$D$75:$D$79</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.44444444444444442</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23863636363636365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3182646133465806E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8229166666666667E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0415-4505-9CF8-5F1822558C11}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cryptopunks!$E$74</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>cryptopunks!$A$75:$A$79</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Alien</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ape</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Zombie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Male</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Female</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cryptopunks!$E$75:$E$79</c:f>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-0415-4505-9CF8-5F1822558C11}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cryptopunks!$F$74</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>cryptopunks!$A$75:$A$79</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Alien</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ape</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Zombie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Male</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Female</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cryptopunks!$F$75:$F$79</c:f>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-0415-4505-9CF8-5F1822558C11}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cryptopunks!$G$74</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>cryptopunks!$A$75:$A$79</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Alien</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ape</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Zombie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Male</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Female</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cryptopunks!$G$75:$G$79</c:f>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-0415-4505-9CF8-5F1822558C11}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cryptopunks!$H$74</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percentage of punk type not in top sales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F496D7"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>cryptopunks!$A$75:$A$79</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Alien</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ape</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Zombie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Male</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Female</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cryptopunks!$H$75:$H$79</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.55555555555555558</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76136363636363635</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99768173538665339</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99817708333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-0415-4505-9CF8-5F1822558C11}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1139390720"/>
+        <c:axId val="1139405696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1139390720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1139405696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1139405696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1139390720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:noFill/>
@@ -4842,7 +6063,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5046,23 +6267,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -5167,8 +6387,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5300,20 +6520,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5347,7 +6566,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5551,23 +6770,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -5672,8 +6890,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5805,20 +7023,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5955,8 +7172,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="219364" y="2282799"/>
-          <a:ext cx="1604818" cy="1088572"/>
+          <a:off x="219364" y="2288242"/>
+          <a:ext cx="1604818" cy="1104900"/>
           <a:chOff x="6021294" y="11586883"/>
           <a:chExt cx="1837850" cy="1234004"/>
         </a:xfrm>
@@ -6115,8 +7332,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2401511" y="2275673"/>
-          <a:ext cx="1605600" cy="1089008"/>
+          <a:off x="2401511" y="2281116"/>
+          <a:ext cx="1605600" cy="1105336"/>
           <a:chOff x="6021297" y="11586883"/>
           <a:chExt cx="1763059" cy="1135530"/>
         </a:xfrm>
@@ -6243,82 +7460,6 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>219728</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>10525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4020657</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>5763</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="15" name="Chart 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F0AE41E-78E7-4D79-B183-EB59B70DD0B1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>219392</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>10153</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4020992</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>7485</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="42" name="Chart 41">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6436C39-2B41-4F2E-8069-E1B52894503B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -6489,8 +7630,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4584440" y="2286872"/>
-          <a:ext cx="1604819" cy="1089008"/>
+          <a:off x="4584440" y="2292315"/>
+          <a:ext cx="1604819" cy="1105336"/>
           <a:chOff x="3635460" y="2163074"/>
           <a:chExt cx="1604819" cy="1121024"/>
         </a:xfrm>
@@ -6687,8 +7828,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="23091" y="680357"/>
-          <a:ext cx="8597435" cy="1397000"/>
+          <a:off x="23091" y="679450"/>
+          <a:ext cx="8598342" cy="1397000"/>
           <a:chOff x="23091" y="679824"/>
           <a:chExt cx="8597968" cy="1397000"/>
         </a:xfrm>
@@ -6707,7 +7848,7 @@
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill rotWithShape="1">
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
             <a:extLst>
               <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
                 <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -6909,8 +8050,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6766588" y="2277635"/>
-          <a:ext cx="1604819" cy="1090337"/>
+          <a:off x="6766588" y="2283078"/>
+          <a:ext cx="1604819" cy="1106665"/>
           <a:chOff x="3635460" y="2163074"/>
           <a:chExt cx="1604819" cy="1122368"/>
         </a:xfrm>
@@ -7249,123 +8390,118 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>208643</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4010243</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>157685</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="29" name="Chart 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4932387-851E-46BF-9156-47745397353E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>216137</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>3550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4017737</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>180167</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="30" name="Chart 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F180D839-E596-4A41-BDCD-DE3E0437E4E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.08346</cdr:x>
-      <cdr:y>0.18357</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.19158</cdr:x>
-      <cdr:y>0.86497</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="4" name="TextBox 3">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4527BD47-6DB3-9110-7B19-28A1229E246D}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="349250" y="468313"/>
-          <a:ext cx="452438" cy="1738312"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.08251</cdr:x>
-      <cdr:y>0.18202</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.19347</cdr:x>
-      <cdr:y>0.86497</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="5" name="TextBox 4">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7466C276-E3B4-CDD1-5058-DBACE7EA3C34}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="345281" y="464344"/>
-          <a:ext cx="464344" cy="1742281"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D5B41EA7-B9F1-45BF-AC06-727F739B53F6}" name="Table1" displayName="Table1" ref="A1:K53" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D5B41EA7-B9F1-45BF-AC06-727F739B53F6}" name="Table1" displayName="Table1" ref="A1:K53" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:K53" xr:uid="{D5B41EA7-B9F1-45BF-AC06-727F739B53F6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K53">
     <sortCondition ref="A1:A61"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{38057EE2-F64A-462F-92E7-FEC2B4F7B8CE}" name="position" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{7B33F43B-E4A0-4577-963E-E7784F5F5010}" name="id" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{4F2F7C75-F344-41BC-A043-C01E3FBCA24D}" name="price_ether" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{E441128D-BBAF-4AFC-BAD7-C05638BEAB26}" name="price_usd" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{26808E42-36A9-41ED-A41F-EFE59547DDF6}" name="Column1" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{2AA96931-7E5F-465F-A96D-8AFCD6B9918D}" name="Column2" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{F002574D-FACF-48C7-8431-D7C24D174487}" name="Column3" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{DBBFAF1B-834A-4E4F-BB32-342BCE3546B1}" name="date_sold" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{38057EE2-F64A-462F-92E7-FEC2B4F7B8CE}" name="position" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{7B33F43B-E4A0-4577-963E-E7784F5F5010}" name="id" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{4F2F7C75-F344-41BC-A043-C01E3FBCA24D}" name="price_ether" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{E441128D-BBAF-4AFC-BAD7-C05638BEAB26}" name="price_usd" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{26808E42-36A9-41ED-A41F-EFE59547DDF6}" name="Column1" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{2AA96931-7E5F-465F-A96D-8AFCD6B9918D}" name="Column2" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{F002574D-FACF-48C7-8431-D7C24D174487}" name="Column3" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{DBBFAF1B-834A-4E4F-BB32-342BCE3546B1}" name="date_sold" dataDxfId="5">
       <calculatedColumnFormula>CONCATENATE(E2, " ", F2, " ", G2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5AEA87E2-6AC8-404A-863B-800A0A13A691}" name="attributes_count" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{9B207B84-3DDB-489A-8C36-B95FEDCCC82F}" name="specific_attribute" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{94169409-101E-443D-A1F9-3E45E94A5462}" name="punk_type" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{5AEA87E2-6AC8-404A-863B-800A0A13A691}" name="attributes_count" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{9B207B84-3DDB-489A-8C36-B95FEDCCC82F}" name="specific_attribute" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{94169409-101E-443D-A1F9-3E45E94A5462}" name="punk_type" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0C6ECD9A-4EBB-4A32-9145-B733F62E8B98}" name="Table2" displayName="Table2" ref="A1:E101" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0C6ECD9A-4EBB-4A32-9145-B733F62E8B98}" name="Table2" displayName="Table2" ref="A1:E101" totalsRowShown="0" headerRowDxfId="1">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E101">
     <sortCondition ref="B1:B101"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{CF5C5033-1551-4011-8DCC-42EA683693B9}" name="attribute"/>
-    <tableColumn id="2" xr3:uid="{E5050196-B703-4DDE-9C04-96F357B01E6D}" name="number_of_punks_with_attribute" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{E5050196-B703-4DDE-9C04-96F357B01E6D}" name="number_of_punks_with_attribute" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{E8D5B3EC-17CA-475A-8372-C6E0FE4EC7CA}" name="availability"/>
     <tableColumn id="4" xr3:uid="{EF888C13-34D9-48BC-9E84-FA4AE88231D2}" name="average_sale (Ξ)"/>
     <tableColumn id="7" xr3:uid="{B8A87290-F75D-4E1A-95AD-CE0367DBEA50}" name="cheapest (Ξ)"/>
@@ -7686,7 +8822,7 @@
       <c r="B2" t="s">
         <v>343</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="19" t="s">
         <v>346</v>
       </c>
     </row>
@@ -7707,8 +8843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6946B6DC-972A-4A33-9276-1E5BC691C458}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7718,7 +8854,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="18" t="s">
         <v>341</v>
       </c>
     </row>
@@ -7734,8 +8870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J76" sqref="J76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7745,45 +8881,45 @@
     <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.1796875" customWidth="1"/>
     <col min="5" max="7" width="10.54296875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="54.36328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="17" t="s">
         <v>95</v>
       </c>
     </row>
@@ -9670,117 +10806,169 @@
       <c r="C63" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D63" s="9" t="s">
         <v>290</v>
       </c>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="6" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="11" t="s">
         <v>202</v>
       </c>
       <c r="B64" s="2">
-        <f xml:space="preserve"> COUNTIF($I$2:$I$61, A64)</f>
+        <f t="shared" ref="B64:B69" si="2" xml:space="preserve"> COUNTIF($I$2:$I$61, A64)</f>
         <v>2</v>
       </c>
       <c r="C64" s="2">
         <f>VLOOKUP(A64, attributes!$A$1:$E$101, 2, FALSE)</f>
         <v>11</v>
       </c>
-      <c r="D64" s="11">
-        <f>B64/C64</f>
+      <c r="D64" s="21">
+        <f t="shared" ref="D64:D69" si="3">B64/C64</f>
         <v>0.18181818181818182</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="23">
+        <f>100% - D64</f>
+        <v>0.81818181818181812</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>196</v>
       </c>
       <c r="B65" s="2">
-        <f xml:space="preserve"> COUNTIF($I$2:$I$61, A65)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C65" s="2">
         <f>VLOOKUP(A65, attributes!$A$1:$E$101, 2, FALSE)</f>
         <v>8</v>
       </c>
-      <c r="D65" s="11">
-        <f>B65/C65</f>
+      <c r="D65" s="21">
+        <f t="shared" si="3"/>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="13" t="s">
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="23">
+        <f t="shared" ref="H65:H70" si="4">100% - D65</f>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" s="11" t="s">
         <v>197</v>
       </c>
       <c r="B66" s="2">
-        <f xml:space="preserve"> COUNTIF($I$2:$I$61, A66)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="C66" s="2">
         <f>VLOOKUP(A66, attributes!$A$1:$E$101, 2, FALSE)</f>
         <v>333</v>
       </c>
-      <c r="D66" s="11">
-        <f>B66/C66</f>
+      <c r="D66" s="21">
+        <f t="shared" si="3"/>
         <v>2.7027027027027029E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="13" t="s">
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="23">
+        <f t="shared" si="4"/>
+        <v>0.97297297297297303</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67" s="11" t="s">
         <v>198</v>
       </c>
       <c r="B67" s="2">
-        <f xml:space="preserve"> COUNTIF($I$2:$I$61, A67)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="C67" s="2">
         <f>VLOOKUP(A67, attributes!$A$1:$E$101, 2, FALSE)</f>
         <v>3560</v>
       </c>
-      <c r="D67" s="11">
-        <f>B67/C67</f>
+      <c r="D67" s="21">
+        <f t="shared" si="3"/>
         <v>5.3370786516853935E-3</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" s="13" t="s">
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="23">
+        <f t="shared" si="4"/>
+        <v>0.99466292134831458</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68" s="11" t="s">
         <v>199</v>
       </c>
       <c r="B68" s="2">
-        <f xml:space="preserve"> COUNTIF($I$2:$I$61, A68)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="C68" s="2">
         <f>VLOOKUP(A68, attributes!$A$1:$E$101, 2, FALSE)</f>
         <v>4501</v>
       </c>
-      <c r="D68" s="11">
-        <f>B68/C68</f>
+      <c r="D68" s="21">
+        <f t="shared" si="3"/>
         <v>4.2212841590757609E-3</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="14" t="s">
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="23">
+        <f t="shared" si="4"/>
+        <v>0.99577871584092426</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="12" t="s">
         <v>200</v>
       </c>
       <c r="B69" s="4">
-        <f xml:space="preserve"> COUNTIF($I$2:$I$61, A69)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C69" s="4">
         <f>VLOOKUP(A69, attributes!$A$1:$E$101, 2, FALSE)</f>
         <v>1420</v>
       </c>
-      <c r="D69" s="12">
-        <f>B69/C69</f>
+      <c r="D69" s="24">
+        <f t="shared" si="3"/>
         <v>1.4084507042253522E-3</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="15"/>
-    </row>
-    <row r="73" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="25">
+        <f t="shared" si="4"/>
+        <v>0.99859154929577465</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="13"/>
+      <c r="H70" s="20">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
         <v>286</v>
       </c>
@@ -9790,11 +10978,17 @@
       <c r="C74" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="D74" s="10" t="s">
+      <c r="D74" s="28" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E74" s="22"/>
+      <c r="F74" s="22"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="10" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
         <v>101</v>
       </c>
@@ -9806,13 +11000,20 @@
         <f>VLOOKUP(A75, attributes!$A$1:$E$101, 2, FALSE)</f>
         <v>9</v>
       </c>
-      <c r="D75" s="11">
+      <c r="D75" s="21">
         <f>B75/C75</f>
         <v>0.44444444444444442</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="23">
+        <f>100% - D75</f>
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76" s="7" t="s">
         <v>102</v>
       </c>
       <c r="B76" s="2">
@@ -9823,12 +11024,19 @@
         <f>VLOOKUP(A76, attributes!$A$1:$E$101, 2, FALSE)</f>
         <v>24</v>
       </c>
-      <c r="D76" s="11">
+      <c r="D76" s="21">
         <f>B76/C76</f>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="23">
+        <f t="shared" ref="H76:H79" si="5">100% - D76</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="7" t="s">
         <v>103</v>
       </c>
@@ -9840,57 +11048,78 @@
         <f>VLOOKUP(A77, attributes!$A$1:$E$101, 2, FALSE)</f>
         <v>88</v>
       </c>
-      <c r="D77" s="11">
+      <c r="D77" s="21">
         <f>B77/C77</f>
         <v>0.23863636363636365</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="23">
+        <f t="shared" si="5"/>
+        <v>0.76136363636363635</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="7" t="s">
         <v>107</v>
       </c>
       <c r="B78" s="2">
-        <f t="shared" ref="B76:B79" si="2">COUNTIF($K$2:$K$61, A78)</f>
+        <f t="shared" ref="B78:B79" si="6">COUNTIF($K$2:$K$61, A78)</f>
         <v>14</v>
       </c>
       <c r="C78" s="2">
         <f>VLOOKUP(A78, attributes!$A$1:$E$101, 2, FALSE)</f>
         <v>6039</v>
       </c>
-      <c r="D78" s="11">
+      <c r="D78" s="21">
         <f>B78/C78</f>
         <v>2.3182646133465806E-3</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="23">
+        <f t="shared" si="5"/>
+        <v>0.99768173538665339</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="8" t="s">
         <v>106</v>
       </c>
       <c r="B79" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="C79" s="4">
         <f>VLOOKUP(A79, attributes!$A$1:$E$101, 2, FALSE)</f>
         <v>3840</v>
       </c>
-      <c r="D79" s="12">
+      <c r="D79" s="24">
         <f>B79/C79</f>
         <v>1.8229166666666667E-3</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="16" t="s">
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="25">
+        <f>100% - D79</f>
+        <v>0.99817708333333333</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="26" t="s">
         <v>289</v>
       </c>
-      <c r="B80" s="17">
+      <c r="B80" s="27">
         <f>SUM(B75:B79)</f>
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B53">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9920,19 +11149,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="14" t="s">
         <v>345</v>
       </c>
     </row>

</xml_diff>